<commit_message>
corregí el dato del 30/07
</commit_message>
<xml_diff>
--- a/datos_dropcontrol/2025-07-30.xlsx
+++ b/datos_dropcontrol/2025-07-30.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\mi-app-humedad\datos_dropcontrol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48AF0705-E9D8-439A-BE0B-490B03E9ED97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF49AA87-7657-4608-9CD8-E075812235C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="390" windowWidth="28800" windowHeight="10125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -96,7 +96,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -153,7 +153,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,7 +459,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,7 +835,7 @@
         <v>74.599999999999994</v>
       </c>
       <c r="E13">
-        <v>9.44</v>
+        <v>79.44</v>
       </c>
       <c r="F13">
         <v>613.48</v>

</xml_diff>